<commit_message>
Üres megyarítás sorok törölve
Üres megyarítás sorok törölve
</commit_message>
<xml_diff>
--- a/xlsx/djangojs-studio.po.xlsx
+++ b/xlsx/djangojs-studio.po.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Translations" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="555" windowWidth="22695" windowHeight="8130"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Translations" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="437">
   <si>
     <t>Message id</t>
   </si>
@@ -582,9 +582,6 @@
     <t>Nincs használatban</t>
   </si>
   <si>
-    <t>Used in %(count)s unit</t>
-  </si>
-  <si>
     <t>This content group is not in use. Add a content group to any unit from the %(outlineAnchor)s.</t>
   </si>
   <si>
@@ -637,9 +634,6 @@
   </si>
   <si>
     <t>Kérlek válassz PDF fájlt a feltöltéshez</t>
-  </si>
-  <si>
-    <t>Contains %(count)s group</t>
   </si>
   <si>
     <t>This Group Configuration is not in use. Start by adding a content experiment to any Unit via the %(outlineAnchor)s.</t>
@@ -1338,20 +1332,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1367,16 +1360,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1664,19 +1662,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96 B106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1692,7 +1687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1700,7 +1695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1708,7 +1703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1716,7 +1711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1724,7 +1719,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1732,7 +1727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1740,7 +1735,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1748,7 +1743,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1756,7 +1751,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1764,7 +1759,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1780,7 +1775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1788,7 +1783,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1796,7 +1791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1804,7 +1799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1812,7 +1807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1820,7 +1815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1828,7 +1823,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1836,7 +1831,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1844,7 +1839,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1852,7 +1847,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1860,7 +1855,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1868,7 +1863,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1876,7 +1871,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1884,7 +1879,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1892,7 +1887,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1900,7 +1895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1908,7 +1903,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1916,7 +1911,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -1924,7 +1919,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -1932,7 +1927,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -1940,7 +1935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1948,7 +1943,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -1956,7 +1951,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -1964,7 +1959,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1972,7 +1967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1980,7 +1975,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1988,7 +1983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>76</v>
       </c>
@@ -1996,7 +1991,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -2004,7 +1999,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -2012,7 +2007,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2020,7 +2015,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2028,7 +2023,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2036,7 +2031,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
@@ -2044,7 +2039,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -2052,7 +2047,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2060,7 +2055,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
@@ -2068,7 +2063,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>96</v>
       </c>
@@ -2076,7 +2071,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
@@ -2084,7 +2079,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
@@ -2092,7 +2087,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -2100,7 +2095,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>104</v>
       </c>
@@ -2108,7 +2103,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
@@ -2116,7 +2111,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -2124,7 +2119,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>110</v>
       </c>
@@ -2132,7 +2127,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -2140,7 +2135,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>114</v>
       </c>
@@ -2148,7 +2143,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>116</v>
       </c>
@@ -2156,7 +2151,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>118</v>
       </c>
@@ -2164,7 +2159,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2172,7 +2167,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -2180,7 +2175,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -2188,7 +2183,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>126</v>
       </c>
@@ -2196,7 +2191,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -2204,7 +2199,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>130</v>
       </c>
@@ -2212,7 +2207,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -2220,7 +2215,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -2228,7 +2223,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -2236,7 +2231,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -2244,7 +2239,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -2252,7 +2247,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2260,7 +2255,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -2268,7 +2263,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -2276,7 +2271,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -2284,7 +2279,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -2292,7 +2287,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -2300,7 +2295,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -2308,7 +2303,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -2316,7 +2311,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -2324,7 +2319,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -2332,7 +2327,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -2340,7 +2335,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -2348,7 +2343,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -2356,7 +2351,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -2364,7 +2359,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -2372,7 +2367,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -2380,7 +2375,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -2388,7 +2383,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -2396,7 +2391,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -2404,7 +2399,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -2412,7 +2407,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -2420,7 +2415,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>184</v>
       </c>
@@ -2428,7 +2423,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -2436,1026 +2431,1015 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>188</v>
       </c>
-      <c r="B96" t="s"/>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="B96" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B97" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B98" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B99" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B100" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B101" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B102" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B103" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B104" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B105" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>207</v>
-      </c>
-      <c r="B106" t="s"/>
-    </row>
-    <row r="107" spans="1:2">
+        <v>208</v>
+      </c>
+      <c r="B106" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B107" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B108" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B109" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B110" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B111" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B112" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B113" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B114" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B115" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B116" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B117" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B118" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B119" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B120" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B121" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B122" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B123" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B124" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B125" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B126" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B127" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B128" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B129" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B130" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B131" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B132" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B133" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B134" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B135" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B136" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B137" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B138" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B139" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B140" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B141" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B142" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B143" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B144" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B145" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B146" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B147" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B148" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B149" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B150" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B151" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B152" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B153" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B154" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B155" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B156" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B157" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B158" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B159" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B160" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B161" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B162" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B163" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B164" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B165" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B166" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B167" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B168" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B169" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B170" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B171" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B172" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B173" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>342</v>
+      </c>
+      <c r="B174" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>344</v>
+      </c>
+      <c r="B175" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>346</v>
+      </c>
+      <c r="B176" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>348</v>
+      </c>
+      <c r="B177" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>350</v>
+      </c>
+      <c r="B178" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>352</v>
+      </c>
+      <c r="B179" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
-      <c r="A174" t="s">
-        <v>340</v>
-      </c>
-      <c r="B174" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2">
-      <c r="A175" t="s">
-        <v>342</v>
-      </c>
-      <c r="B175" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2">
-      <c r="A176" t="s">
-        <v>344</v>
-      </c>
-      <c r="B176" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
-      <c r="A177" t="s">
-        <v>346</v>
-      </c>
-      <c r="B177" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
-      <c r="A178" t="s">
-        <v>348</v>
-      </c>
-      <c r="B178" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2">
-      <c r="A179" t="s">
-        <v>350</v>
-      </c>
-      <c r="B179" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B180" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B181" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B182" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B183" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B184" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B185" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B186" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B187" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B188" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B189" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B190" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B191" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B192" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B193" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B194" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B195" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B196" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B197" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B198" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B199" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B200" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B201" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B202" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B203" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B204" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B205" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B206" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B207" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B208" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B209" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B210" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B211" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B212" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B213" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B214" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B215" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B216" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B217" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B218" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B219" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B220" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B221" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2">
-      <c r="A222" t="s">
-        <v>435</v>
-      </c>
-      <c r="B222" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
-      <c r="A223" t="s">
-        <v>437</v>
-      </c>
-      <c r="B223" t="s">
-        <v>438</v>
-      </c>
-    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>